<commit_message>
Add users to group
Function createUsersFromExcel() is no functional
Note: testing needs to be done with a excel containing at least one
user that’s among the first 100 ArcGIS Online users of the portal,
since a bug prevents getting more then 100 users
</commit_message>
<xml_diff>
--- a/files/exampleUsersGroups.xlsx
+++ b/files/exampleUsersGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="16040" windowHeight="15200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>Leerlingachternaam2</t>
   </si>
   <si>
-    <t>leerling1_schoolnaam</t>
-  </si>
-  <si>
     <t>leerling2_schoolnaam</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>leerling3_schoolnaam</t>
+  </si>
+  <si>
+    <t>34895_develstein</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -471,7 +471,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -494,7 +494,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -508,16 +508,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>

</xml_diff>